<commit_message>
Added Stocks Quantity and Excel Import
</commit_message>
<xml_diff>
--- a/public/Material_Registration.xlsx
+++ b/public/Material_Registration.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mims\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aims\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22635" windowHeight="11025" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22635" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Material Registration" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +177,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -210,6 +218,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,48 +507,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -546,6 +562,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -589,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added designations, UOMS and label on withdrawal
</commit_message>
<xml_diff>
--- a/public/Material_Registration.xlsx
+++ b/public/Material_Registration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Part Number</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>MASMO1 (T00008)</t>
+  </si>
+  <si>
+    <t>Maintenance Supervisor</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +589,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Data Management'!$E$1:$E$2</xm:f>
+            <xm:f>'Data Management'!$E$1:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -607,7 +610,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,6 +664,9 @@
       <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">

</xml_diff>